<commit_message>
updated model performance summary with PV experiment
</commit_message>
<xml_diff>
--- a/plots/model_performance_comparison.xlsx
+++ b/plots/model_performance_comparison.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethbrasseale/Projects/eDNA/code/R/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC22BB-0360-2E44-921B-702FC2A77A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8873FD83-67FB-BD45-9103-958E588FA363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{BC6E49AD-47D7-F249-BF80-8BE9CE838060}"/>
+    <workbookView xWindow="3840" yWindow="2200" windowWidth="28040" windowHeight="15980" xr2:uid="{BC6E49AD-47D7-F249-BF80-8BE9CE838060}"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" sheetId="1" r:id="rId1"/>
-    <sheet name="priors" sheetId="2" r:id="rId2"/>
+    <sheet name="proc var summary" sheetId="3" r:id="rId1"/>
+    <sheet name="summary" sheetId="1" r:id="rId2"/>
+    <sheet name="priors" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
   <si>
     <t>model name</t>
   </si>
@@ -154,6 +155,21 @@
   </si>
   <si>
     <t>lower=0, upper=1</t>
+  </si>
+  <si>
+    <t>waic</t>
+  </si>
+  <si>
+    <t>looic</t>
+  </si>
+  <si>
+    <t>σ_w</t>
+  </si>
+  <si>
+    <t>WAIC</t>
+  </si>
+  <si>
+    <t>LOO IC</t>
   </si>
 </sst>
 </file>
@@ -189,11 +205,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -212,9 +229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -252,7 +269,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -358,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -500,18 +517,391 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64644ADB-F159-824E-8CB1-3FC7B4EDF34F}">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1.24</v>
+      </c>
+      <c r="F2">
+        <v>0.31459999999999999</v>
+      </c>
+      <c r="G2">
+        <v>382.733</v>
+      </c>
+      <c r="J2">
+        <v>681.63499999999999</v>
+      </c>
+      <c r="K2">
+        <v>685.5</v>
+      </c>
+      <c r="L2">
+        <v>675.75</v>
+      </c>
+      <c r="M2">
+        <v>0.8135</v>
+      </c>
+      <c r="N2">
+        <v>279.89999999999998</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>1.28</v>
+      </c>
+      <c r="F3">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="G3">
+        <v>435.315</v>
+      </c>
+      <c r="J3">
+        <v>574.07600000000002</v>
+      </c>
+      <c r="K3">
+        <v>685.59</v>
+      </c>
+      <c r="L3">
+        <v>675.51</v>
+      </c>
+      <c r="M3">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="N3">
+        <v>275.39999999999998</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1.7E-15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="F4">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="G4">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="H4">
+        <v>7135.75</v>
+      </c>
+      <c r="J4">
+        <v>163.83000000000001</v>
+      </c>
+      <c r="K4">
+        <v>638.19000000000005</v>
+      </c>
+      <c r="L4">
+        <v>631.54999999999995</v>
+      </c>
+      <c r="M4">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="N4">
+        <v>199.5</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>0.85</v>
+      </c>
+      <c r="F5">
+        <v>0.1186</v>
+      </c>
+      <c r="G5">
+        <v>212.47800000000001</v>
+      </c>
+      <c r="H5">
+        <v>61830.879999999997</v>
+      </c>
+      <c r="J5">
+        <v>118.75</v>
+      </c>
+      <c r="K5">
+        <v>620.9</v>
+      </c>
+      <c r="L5">
+        <v>618.84</v>
+      </c>
+      <c r="M5">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="N5">
+        <v>171.4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>1.274</v>
+      </c>
+      <c r="F6">
+        <v>0.24990000000000001</v>
+      </c>
+      <c r="G6">
+        <v>381</v>
+      </c>
+      <c r="I6">
+        <v>7.22</v>
+      </c>
+      <c r="J6">
+        <v>608.95000000000005</v>
+      </c>
+      <c r="K6">
+        <v>685.11</v>
+      </c>
+      <c r="L6">
+        <v>676.97</v>
+      </c>
+      <c r="M6">
+        <v>0.58069999999999999</v>
+      </c>
+      <c r="N6">
+        <v>437.5</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2.7590000000000001E-9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>0.73580000000000001</v>
+      </c>
+      <c r="F7">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G7">
+        <v>79.59</v>
+      </c>
+      <c r="H7">
+        <v>7069.549</v>
+      </c>
+      <c r="I7">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="J7">
+        <v>170.78</v>
+      </c>
+      <c r="K7">
+        <v>639.69000000000005</v>
+      </c>
+      <c r="L7">
+        <v>633.16</v>
+      </c>
+      <c r="M7">
+        <v>0.9829</v>
+      </c>
+      <c r="N7">
+        <v>207</v>
+      </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="F8">
+        <v>0.1191</v>
+      </c>
+      <c r="G8">
+        <v>208.9</v>
+      </c>
+      <c r="H8">
+        <v>62512.69</v>
+      </c>
+      <c r="I8">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="J8">
+        <v>117.62</v>
+      </c>
+      <c r="K8">
+        <v>620.20000000000005</v>
+      </c>
+      <c r="L8">
+        <v>617.66200000000003</v>
+      </c>
+      <c r="M8">
+        <v>0.97729999999999995</v>
+      </c>
+      <c r="N8">
+        <v>195.5</v>
+      </c>
+      <c r="O8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A10F6E-60C2-D34D-AEF9-61F026003DBC}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,10 +914,12 @@
     <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -556,19 +948,25 @@
         <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -597,16 +995,22 @@
         <v>26</v>
       </c>
       <c r="J2">
+        <v>806.1</v>
+      </c>
+      <c r="K2">
+        <v>801.2</v>
+      </c>
+      <c r="L2">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>3810</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>0.35499999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -635,16 +1039,22 @@
         <v>26</v>
       </c>
       <c r="J3">
+        <v>743.9</v>
+      </c>
+      <c r="K3">
+        <v>745</v>
+      </c>
+      <c r="L3">
         <v>0.25559999999999999</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>3282</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -673,16 +1083,22 @@
         <v>26</v>
       </c>
       <c r="J4">
+        <v>637.6</v>
+      </c>
+      <c r="K4">
+        <v>641.1</v>
+      </c>
+      <c r="L4">
         <v>0.93500000000000005</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>970</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -711,16 +1127,22 @@
         <v>26</v>
       </c>
       <c r="J5">
+        <v>616.70000000000005</v>
+      </c>
+      <c r="K5">
+        <v>619.4</v>
+      </c>
+      <c r="L5">
         <v>0.93</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>1004</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -749,16 +1171,22 @@
         <v>-8.9</v>
       </c>
       <c r="J6">
+        <v>786.2</v>
+      </c>
+      <c r="K6">
+        <v>781.1</v>
+      </c>
+      <c r="L6">
         <v>-0.02</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>3845</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>0.73499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -787,16 +1215,22 @@
         <v>-1.4</v>
       </c>
       <c r="J7">
+        <v>639.1</v>
+      </c>
+      <c r="K7">
+        <v>643.29999999999995</v>
+      </c>
+      <c r="L7">
         <v>0.95489999999999997</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>817</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -825,12 +1259,18 @@
         <v>-1.1000000000000001</v>
       </c>
       <c r="J8">
+        <v>616.70000000000005</v>
+      </c>
+      <c r="K8">
+        <v>620</v>
+      </c>
+      <c r="L8">
         <v>0.94930000000000003</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>856</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -839,12 +1279,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690ECE77-C7E0-364C-A099-061D4F4F36C2}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,7 +1367,15 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>